<commit_message>
orange dot draft updates
</commit_message>
<xml_diff>
--- a/pieCharts.xlsx
+++ b/pieCharts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Desktop/Equity Center/orange-dot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B905E8C0-EB5C-AB48-9A20-565E6E1B59CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A13E7E-0D6C-4A4D-8D27-F1A93D54F38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6840" yWindow="500" windowWidth="21020" windowHeight="15920" xr2:uid="{C0AF3331-2210-A546-8BED-F18C12237DF8}"/>
   </bookViews>
@@ -324,8 +324,21 @@
                           <a:schemeClr val="bg1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>Self-Sufficient</a:t>
+                      <a:t>Paid</a:t>
                     </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> a living wage</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1800">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
                   </a:p>
                   <a:p>
                     <a:pPr>
@@ -412,8 +425,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15150889954467445"/>
-                  <c:y val="-0.12265091863517061"/>
+                  <c:x val="0.14442089009399511"/>
+                  <c:y val="-0.11415834963304747"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -434,12 +447,8 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0"/>
-                      <a:t>Likely able</a:t>
-                    </a:r>
-                    <a:r>
                       <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t> to </a:t>
+                      <a:t>Paid close to </a:t>
                     </a:r>
                   </a:p>
                   <a:p>
@@ -452,33 +461,7 @@
                     </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t>earn their </a:t>
-                    </a:r>
-                  </a:p>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1400">
-                        <a:solidFill>
-                          <a:schemeClr val="bg1"/>
-                        </a:solidFill>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t>way out of </a:t>
-                    </a:r>
-                  </a:p>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1400">
-                        <a:solidFill>
-                          <a:schemeClr val="bg1"/>
-                        </a:solidFill>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t>poverty</a:t>
+                      <a:t>a living wage</a:t>
                     </a:r>
                   </a:p>
                   <a:p>
@@ -647,7 +630,7 @@
                     </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" sz="1600"/>
-                      <a:t>Not</a:t>
+                      <a:t>Not paid</a:t>
                     </a:r>
                   </a:p>
                   <a:p>
@@ -659,9 +642,10 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1600"/>
-                      <a:t>Self-Sufficient</a:t>
+                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                      <a:t>a living wage</a:t>
                     </a:r>
+                    <a:endParaRPr lang="en-US" sz="1600"/>
                   </a:p>
                   <a:p>
                     <a:pPr>
@@ -1537,15 +1521,23 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Not likely</a:t>
+            <a:t>Not paid</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> able to </a:t>
+            <a:t>close to a </a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -1556,7 +1548,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>earn their way out of poverty</a:t>
+            <a:t>living wage</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -1869,7 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F15CAED-2C58-D645-85DF-78D0186DA637}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
locality profiles language in progress
</commit_message>
<xml_diff>
--- a/pieCharts.xlsx
+++ b/pieCharts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Desktop/Equity Center/orange-dot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A13E7E-0D6C-4A4D-8D27-F1A93D54F38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F620F3D4-D285-4446-9B2C-E6D8EAF4B8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6840" yWindow="500" windowWidth="21020" windowHeight="15920" xr2:uid="{C0AF3331-2210-A546-8BED-F18C12237DF8}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F15CAED-2C58-D645-85DF-78D0186DA637}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>

</xml_diff>